<commit_message>
update report for vref=250mV
</commit_message>
<xml_diff>
--- a/dcd_compsr_offset_tran_tsmc2p_meas.xlsx
+++ b/dcd_compsr_offset_tran_tsmc2p_meas.xlsx
@@ -1032,13 +1032,13 @@
         <v>36</v>
       </c>
       <c r="R2">
-        <v>349.628</v>
+        <v>250.514</v>
       </c>
       <c r="S2">
-        <v>-0.371939</v>
+        <v>-99.48650000000001</v>
       </c>
       <c r="T2">
-        <v>-0.371939</v>
+        <v>-0.513522</v>
       </c>
       <c r="U2" s="2" t="s">
         <v>37</v>
@@ -1227,13 +1227,13 @@
         <v>63</v>
       </c>
       <c r="R5">
-        <v>314.555</v>
+        <v>250.743</v>
       </c>
       <c r="S5">
-        <v>-0.44543</v>
+        <v>-64.2572</v>
       </c>
       <c r="T5">
-        <v>-0.44543</v>
+        <v>-0.742795</v>
       </c>
       <c r="U5" s="2" t="s">
         <v>37</v>
@@ -1292,13 +1292,13 @@
         <v>63</v>
       </c>
       <c r="R6">
-        <v>314.882</v>
+        <v>267.523</v>
       </c>
       <c r="S6">
-        <v>-0.118</v>
+        <v>-47.4774</v>
       </c>
       <c r="T6">
-        <v>-0.118</v>
+        <v>-17.5226</v>
       </c>
       <c r="U6" s="2" t="s">
         <v>37</v>
@@ -7679,13 +7679,13 @@
         <v>170</v>
       </c>
       <c r="R105" s="1">
-        <v>314.555</v>
+        <v>250.514</v>
       </c>
       <c r="S105" s="1">
-        <v>-0.44543</v>
+        <v>-99.48650000000001</v>
       </c>
       <c r="T105" s="1">
-        <v>-0.44543</v>
+        <v>-17.5226</v>
       </c>
       <c r="U105" s="1" t="s">
         <v>50</v>
@@ -7696,13 +7696,13 @@
         <v>171</v>
       </c>
       <c r="R106" s="1">
-        <v>349.628</v>
+        <v>267.523</v>
       </c>
       <c r="S106" s="1">
-        <v>-0.118</v>
+        <v>-47.4774</v>
       </c>
       <c r="T106" s="1">
-        <v>-0.118</v>
+        <v>-0.513522</v>
       </c>
       <c r="U106" s="1" t="s">
         <v>50</v>
@@ -7733,13 +7733,13 @@
         <v>176</v>
       </c>
       <c r="R111" s="1">
-        <v>326.355</v>
+        <v>256.26</v>
       </c>
       <c r="S111" s="1">
-        <v>-0.3117897</v>
+        <v>-70.40703000000001</v>
       </c>
       <c r="T111" s="1">
-        <v>-0.3117897</v>
+        <v>-6.259639</v>
       </c>
       <c r="U111" s="1" t="s">
         <v>50</v>
@@ -7750,13 +7750,13 @@
         <v>177</v>
       </c>
       <c r="R112" s="1">
-        <v>16.457038</v>
+        <v>7.964692</v>
       </c>
       <c r="S112" s="1">
-        <v>0.140276</v>
+        <v>21.673362</v>
       </c>
       <c r="T112" s="1">
-        <v>0.140276</v>
+        <v>7.964666</v>
       </c>
       <c r="U112" s="1" t="s">
         <v>50</v>
@@ -7767,13 +7767,13 @@
         <v>178</v>
       </c>
       <c r="R113" s="1">
-        <v>5.04268</v>
+        <v>3.108051</v>
       </c>
       <c r="S113" s="1">
-        <v>44.990582</v>
+        <v>30.782952</v>
       </c>
       <c r="T113" s="1">
-        <v>44.990582</v>
+        <v>127.238424</v>
       </c>
       <c r="U113" s="1" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
'change device to elvt'
</commit_message>
<xml_diff>
--- a/dcd_compsr_offset_tran_tsmc2p_meas.xlsx
+++ b/dcd_compsr_offset_tran_tsmc2p_meas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3766" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5602" uniqueCount="233">
   <si>
     <t>Process</t>
   </si>
@@ -106,7 +106,7 @@
     <t>25</t>
   </si>
   <si>
-    <t>0.45</t>
+    <t>0.42</t>
   </si>
   <si>
     <t>0.70</t>
@@ -157,7 +157,7 @@
     <t>125</t>
   </si>
   <si>
-    <t>0.473</t>
+    <t>0.441</t>
   </si>
   <si>
     <t>0.77</t>
@@ -199,7 +199,7 @@
     <t>cap_h</t>
   </si>
   <si>
-    <t>0.414</t>
+    <t>0.386</t>
   </si>
   <si>
     <t>0.63</t>
@@ -376,15 +376,24 @@
     <t>tsmc2p (51)</t>
   </si>
   <si>
+    <t>0.8</t>
+  </si>
+  <si>
     <t>tsmc2p (52)</t>
   </si>
   <si>
+    <t>0.848</t>
+  </si>
+  <si>
     <t>tsmc2p (53)</t>
   </si>
   <si>
     <t>tsmc2p (54)</t>
   </si>
   <si>
+    <t>0.736</t>
+  </si>
+  <si>
     <t>tsmc2p (55)</t>
   </si>
   <si>
@@ -524,6 +533,159 @@
   </si>
   <si>
     <t>tsmc2p (101)</t>
+  </si>
+  <si>
+    <t>tsmc2p (102)</t>
+  </si>
+  <si>
+    <t>tsmc2p (103)</t>
+  </si>
+  <si>
+    <t>tsmc2p (104)</t>
+  </si>
+  <si>
+    <t>tsmc2p (105)</t>
+  </si>
+  <si>
+    <t>tsmc2p (106)</t>
+  </si>
+  <si>
+    <t>tsmc2p (107)</t>
+  </si>
+  <si>
+    <t>tsmc2p (108)</t>
+  </si>
+  <si>
+    <t>tsmc2p (109)</t>
+  </si>
+  <si>
+    <t>tsmc2p (110)</t>
+  </si>
+  <si>
+    <t>tsmc2p (111)</t>
+  </si>
+  <si>
+    <t>tsmc2p (112)</t>
+  </si>
+  <si>
+    <t>tsmc2p (113)</t>
+  </si>
+  <si>
+    <t>tsmc2p (114)</t>
+  </si>
+  <si>
+    <t>tsmc2p (115)</t>
+  </si>
+  <si>
+    <t>tsmc2p (116)</t>
+  </si>
+  <si>
+    <t>tsmc2p (117)</t>
+  </si>
+  <si>
+    <t>tsmc2p (118)</t>
+  </si>
+  <si>
+    <t>tsmc2p (119)</t>
+  </si>
+  <si>
+    <t>tsmc2p (120)</t>
+  </si>
+  <si>
+    <t>tsmc2p (121)</t>
+  </si>
+  <si>
+    <t>tsmc2p (122)</t>
+  </si>
+  <si>
+    <t>tsmc2p (123)</t>
+  </si>
+  <si>
+    <t>tsmc2p (124)</t>
+  </si>
+  <si>
+    <t>tsmc2p (125)</t>
+  </si>
+  <si>
+    <t>tsmc2p (126)</t>
+  </si>
+  <si>
+    <t>tsmc2p (127)</t>
+  </si>
+  <si>
+    <t>tsmc2p (128)</t>
+  </si>
+  <si>
+    <t>tsmc2p (129)</t>
+  </si>
+  <si>
+    <t>tsmc2p (130)</t>
+  </si>
+  <si>
+    <t>tsmc2p (131)</t>
+  </si>
+  <si>
+    <t>tsmc2p (132)</t>
+  </si>
+  <si>
+    <t>tsmc2p (133)</t>
+  </si>
+  <si>
+    <t>tsmc2p (134)</t>
+  </si>
+  <si>
+    <t>tsmc2p (135)</t>
+  </si>
+  <si>
+    <t>tsmc2p (136)</t>
+  </si>
+  <si>
+    <t>tsmc2p (137)</t>
+  </si>
+  <si>
+    <t>tsmc2p (138)</t>
+  </si>
+  <si>
+    <t>tsmc2p (139)</t>
+  </si>
+  <si>
+    <t>tsmc2p (140)</t>
+  </si>
+  <si>
+    <t>tsmc2p (141)</t>
+  </si>
+  <si>
+    <t>tsmc2p (142)</t>
+  </si>
+  <si>
+    <t>tsmc2p (143)</t>
+  </si>
+  <si>
+    <t>tsmc2p (144)</t>
+  </si>
+  <si>
+    <t>tsmc2p (145)</t>
+  </si>
+  <si>
+    <t>tsmc2p (146)</t>
+  </si>
+  <si>
+    <t>tsmc2p (147)</t>
+  </si>
+  <si>
+    <t>tsmc2p (148)</t>
+  </si>
+  <si>
+    <t>tsmc2p (149)</t>
+  </si>
+  <si>
+    <t>tsmc2p (150)</t>
+  </si>
+  <si>
+    <t>tsmc2p (151)</t>
+  </si>
+  <si>
+    <t>tsmc2p (152)</t>
   </si>
   <si>
     <t>Min</t>
@@ -905,13 +1067,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U114"/>
+  <dimension ref="A1:U165"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="113" width="9.140625"/>
+    <col min="1" max="164" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="1" customFormat="1">
@@ -4323,7 +4485,7 @@
         <v>29</v>
       </c>
       <c r="J53" t="s">
-        <v>31</v>
+        <v>120</v>
       </c>
       <c r="K53" t="s">
         <v>31</v>
@@ -4361,7 +4523,7 @@
     </row>
     <row r="54" spans="1:21">
       <c r="A54" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B54" t="s">
         <v>39</v>
@@ -4388,7 +4550,7 @@
         <v>46</v>
       </c>
       <c r="J54" t="s">
-        <v>48</v>
+        <v>122</v>
       </c>
       <c r="K54" t="s">
         <v>48</v>
@@ -4426,7 +4588,7 @@
     </row>
     <row r="55" spans="1:21">
       <c r="A55" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B55" t="s">
         <v>39</v>
@@ -4453,7 +4615,7 @@
         <v>52</v>
       </c>
       <c r="J55" t="s">
-        <v>48</v>
+        <v>122</v>
       </c>
       <c r="K55" t="s">
         <v>48</v>
@@ -4491,7 +4653,7 @@
     </row>
     <row r="56" spans="1:21">
       <c r="A56" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B56" t="s">
         <v>54</v>
@@ -4518,7 +4680,7 @@
         <v>46</v>
       </c>
       <c r="J56" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K56" t="s">
         <v>62</v>
@@ -4556,7 +4718,7 @@
     </row>
     <row r="57" spans="1:21">
       <c r="A57" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B57" t="s">
         <v>54</v>
@@ -4583,7 +4745,7 @@
         <v>52</v>
       </c>
       <c r="J57" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K57" t="s">
         <v>62</v>
@@ -4621,7 +4783,7 @@
     </row>
     <row r="58" spans="1:21">
       <c r="A58" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B58" t="s">
         <v>66</v>
@@ -4648,7 +4810,7 @@
         <v>46</v>
       </c>
       <c r="J58" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K58" t="s">
         <v>62</v>
@@ -4686,7 +4848,7 @@
     </row>
     <row r="59" spans="1:21">
       <c r="A59" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B59" t="s">
         <v>66</v>
@@ -4713,7 +4875,7 @@
         <v>52</v>
       </c>
       <c r="J59" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K59" t="s">
         <v>62</v>
@@ -4751,7 +4913,7 @@
     </row>
     <row r="60" spans="1:21">
       <c r="A60" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B60" t="s">
         <v>72</v>
@@ -4778,7 +4940,7 @@
         <v>46</v>
       </c>
       <c r="J60" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K60" t="s">
         <v>62</v>
@@ -4816,7 +4978,7 @@
     </row>
     <row r="61" spans="1:21">
       <c r="A61" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B61" t="s">
         <v>72</v>
@@ -4843,7 +5005,7 @@
         <v>52</v>
       </c>
       <c r="J61" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K61" t="s">
         <v>62</v>
@@ -4881,7 +5043,7 @@
     </row>
     <row r="62" spans="1:21">
       <c r="A62" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B62" t="s">
         <v>39</v>
@@ -4908,7 +5070,7 @@
         <v>46</v>
       </c>
       <c r="J62" t="s">
-        <v>48</v>
+        <v>122</v>
       </c>
       <c r="K62" t="s">
         <v>48</v>
@@ -4946,7 +5108,7 @@
     </row>
     <row r="63" spans="1:21">
       <c r="A63" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B63" t="s">
         <v>39</v>
@@ -4973,7 +5135,7 @@
         <v>46</v>
       </c>
       <c r="J63" t="s">
-        <v>48</v>
+        <v>122</v>
       </c>
       <c r="K63" t="s">
         <v>48</v>
@@ -5011,7 +5173,7 @@
     </row>
     <row r="64" spans="1:21">
       <c r="A64" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B64" t="s">
         <v>39</v>
@@ -5038,7 +5200,7 @@
         <v>46</v>
       </c>
       <c r="J64" t="s">
-        <v>48</v>
+        <v>122</v>
       </c>
       <c r="K64" t="s">
         <v>48</v>
@@ -5076,7 +5238,7 @@
     </row>
     <row r="65" spans="1:21">
       <c r="A65" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B65" t="s">
         <v>39</v>
@@ -5103,7 +5265,7 @@
         <v>52</v>
       </c>
       <c r="J65" t="s">
-        <v>48</v>
+        <v>122</v>
       </c>
       <c r="K65" t="s">
         <v>48</v>
@@ -5141,7 +5303,7 @@
     </row>
     <row r="66" spans="1:21">
       <c r="A66" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B66" t="s">
         <v>39</v>
@@ -5168,7 +5330,7 @@
         <v>52</v>
       </c>
       <c r="J66" t="s">
-        <v>48</v>
+        <v>122</v>
       </c>
       <c r="K66" t="s">
         <v>48</v>
@@ -5206,7 +5368,7 @@
     </row>
     <row r="67" spans="1:21">
       <c r="A67" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B67" t="s">
         <v>39</v>
@@ -5233,7 +5395,7 @@
         <v>52</v>
       </c>
       <c r="J67" t="s">
-        <v>48</v>
+        <v>122</v>
       </c>
       <c r="K67" t="s">
         <v>48</v>
@@ -5271,7 +5433,7 @@
     </row>
     <row r="68" spans="1:21">
       <c r="A68" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B68" t="s">
         <v>54</v>
@@ -5298,7 +5460,7 @@
         <v>46</v>
       </c>
       <c r="J68" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K68" t="s">
         <v>62</v>
@@ -5336,7 +5498,7 @@
     </row>
     <row r="69" spans="1:21">
       <c r="A69" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B69" t="s">
         <v>54</v>
@@ -5363,7 +5525,7 @@
         <v>46</v>
       </c>
       <c r="J69" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K69" t="s">
         <v>62</v>
@@ -5401,7 +5563,7 @@
     </row>
     <row r="70" spans="1:21">
       <c r="A70" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B70" t="s">
         <v>54</v>
@@ -5428,7 +5590,7 @@
         <v>46</v>
       </c>
       <c r="J70" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K70" t="s">
         <v>62</v>
@@ -5466,7 +5628,7 @@
     </row>
     <row r="71" spans="1:21">
       <c r="A71" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B71" t="s">
         <v>54</v>
@@ -5493,7 +5655,7 @@
         <v>52</v>
       </c>
       <c r="J71" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K71" t="s">
         <v>62</v>
@@ -5531,7 +5693,7 @@
     </row>
     <row r="72" spans="1:21">
       <c r="A72" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B72" t="s">
         <v>54</v>
@@ -5558,7 +5720,7 @@
         <v>52</v>
       </c>
       <c r="J72" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K72" t="s">
         <v>62</v>
@@ -5596,7 +5758,7 @@
     </row>
     <row r="73" spans="1:21">
       <c r="A73" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B73" t="s">
         <v>54</v>
@@ -5623,7 +5785,7 @@
         <v>52</v>
       </c>
       <c r="J73" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K73" t="s">
         <v>62</v>
@@ -5661,7 +5823,7 @@
     </row>
     <row r="74" spans="1:21">
       <c r="A74" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B74" t="s">
         <v>54</v>
@@ -5688,7 +5850,7 @@
         <v>46</v>
       </c>
       <c r="J74" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K74" t="s">
         <v>62</v>
@@ -5726,7 +5888,7 @@
     </row>
     <row r="75" spans="1:21">
       <c r="A75" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B75" t="s">
         <v>54</v>
@@ -5753,7 +5915,7 @@
         <v>46</v>
       </c>
       <c r="J75" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K75" t="s">
         <v>62</v>
@@ -5791,7 +5953,7 @@
     </row>
     <row r="76" spans="1:21">
       <c r="A76" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B76" t="s">
         <v>54</v>
@@ -5818,7 +5980,7 @@
         <v>46</v>
       </c>
       <c r="J76" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K76" t="s">
         <v>62</v>
@@ -5856,7 +6018,7 @@
     </row>
     <row r="77" spans="1:21">
       <c r="A77" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B77" t="s">
         <v>54</v>
@@ -5883,7 +6045,7 @@
         <v>52</v>
       </c>
       <c r="J77" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K77" t="s">
         <v>62</v>
@@ -5921,7 +6083,7 @@
     </row>
     <row r="78" spans="1:21">
       <c r="A78" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B78" t="s">
         <v>54</v>
@@ -5948,7 +6110,7 @@
         <v>52</v>
       </c>
       <c r="J78" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K78" t="s">
         <v>62</v>
@@ -5986,7 +6148,7 @@
     </row>
     <row r="79" spans="1:21">
       <c r="A79" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B79" t="s">
         <v>54</v>
@@ -6013,7 +6175,7 @@
         <v>52</v>
       </c>
       <c r="J79" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K79" t="s">
         <v>62</v>
@@ -6051,7 +6213,7 @@
     </row>
     <row r="80" spans="1:21">
       <c r="A80" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B80" t="s">
         <v>66</v>
@@ -6078,7 +6240,7 @@
         <v>46</v>
       </c>
       <c r="J80" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K80" t="s">
         <v>62</v>
@@ -6116,7 +6278,7 @@
     </row>
     <row r="81" spans="1:21">
       <c r="A81" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B81" t="s">
         <v>66</v>
@@ -6143,7 +6305,7 @@
         <v>46</v>
       </c>
       <c r="J81" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K81" t="s">
         <v>62</v>
@@ -6181,7 +6343,7 @@
     </row>
     <row r="82" spans="1:21">
       <c r="A82" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B82" t="s">
         <v>66</v>
@@ -6208,7 +6370,7 @@
         <v>46</v>
       </c>
       <c r="J82" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K82" t="s">
         <v>62</v>
@@ -6246,7 +6408,7 @@
     </row>
     <row r="83" spans="1:21">
       <c r="A83" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B83" t="s">
         <v>66</v>
@@ -6273,7 +6435,7 @@
         <v>52</v>
       </c>
       <c r="J83" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K83" t="s">
         <v>62</v>
@@ -6311,7 +6473,7 @@
     </row>
     <row r="84" spans="1:21">
       <c r="A84" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B84" t="s">
         <v>66</v>
@@ -6338,7 +6500,7 @@
         <v>52</v>
       </c>
       <c r="J84" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K84" t="s">
         <v>62</v>
@@ -6376,7 +6538,7 @@
     </row>
     <row r="85" spans="1:21">
       <c r="A85" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B85" t="s">
         <v>66</v>
@@ -6403,7 +6565,7 @@
         <v>52</v>
       </c>
       <c r="J85" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K85" t="s">
         <v>62</v>
@@ -6441,7 +6603,7 @@
     </row>
     <row r="86" spans="1:21">
       <c r="A86" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B86" t="s">
         <v>66</v>
@@ -6468,7 +6630,7 @@
         <v>46</v>
       </c>
       <c r="J86" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K86" t="s">
         <v>62</v>
@@ -6506,7 +6668,7 @@
     </row>
     <row r="87" spans="1:21">
       <c r="A87" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B87" t="s">
         <v>66</v>
@@ -6533,7 +6695,7 @@
         <v>46</v>
       </c>
       <c r="J87" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K87" t="s">
         <v>62</v>
@@ -6571,7 +6733,7 @@
     </row>
     <row r="88" spans="1:21">
       <c r="A88" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B88" t="s">
         <v>66</v>
@@ -6598,7 +6760,7 @@
         <v>46</v>
       </c>
       <c r="J88" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K88" t="s">
         <v>62</v>
@@ -6636,7 +6798,7 @@
     </row>
     <row r="89" spans="1:21">
       <c r="A89" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B89" t="s">
         <v>66</v>
@@ -6663,7 +6825,7 @@
         <v>52</v>
       </c>
       <c r="J89" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K89" t="s">
         <v>62</v>
@@ -6701,7 +6863,7 @@
     </row>
     <row r="90" spans="1:21">
       <c r="A90" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B90" t="s">
         <v>66</v>
@@ -6728,7 +6890,7 @@
         <v>52</v>
       </c>
       <c r="J90" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K90" t="s">
         <v>62</v>
@@ -6766,7 +6928,7 @@
     </row>
     <row r="91" spans="1:21">
       <c r="A91" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B91" t="s">
         <v>66</v>
@@ -6793,7 +6955,7 @@
         <v>52</v>
       </c>
       <c r="J91" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K91" t="s">
         <v>62</v>
@@ -6831,7 +6993,7 @@
     </row>
     <row r="92" spans="1:21">
       <c r="A92" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B92" t="s">
         <v>72</v>
@@ -6858,7 +7020,7 @@
         <v>46</v>
       </c>
       <c r="J92" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K92" t="s">
         <v>62</v>
@@ -6896,7 +7058,7 @@
     </row>
     <row r="93" spans="1:21">
       <c r="A93" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B93" t="s">
         <v>72</v>
@@ -6923,7 +7085,7 @@
         <v>46</v>
       </c>
       <c r="J93" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K93" t="s">
         <v>62</v>
@@ -6961,7 +7123,7 @@
     </row>
     <row r="94" spans="1:21">
       <c r="A94" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B94" t="s">
         <v>72</v>
@@ -6988,7 +7150,7 @@
         <v>46</v>
       </c>
       <c r="J94" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K94" t="s">
         <v>62</v>
@@ -7026,7 +7188,7 @@
     </row>
     <row r="95" spans="1:21">
       <c r="A95" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B95" t="s">
         <v>72</v>
@@ -7053,7 +7215,7 @@
         <v>52</v>
       </c>
       <c r="J95" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K95" t="s">
         <v>62</v>
@@ -7091,7 +7253,7 @@
     </row>
     <row r="96" spans="1:21">
       <c r="A96" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B96" t="s">
         <v>72</v>
@@ -7118,7 +7280,7 @@
         <v>52</v>
       </c>
       <c r="J96" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K96" t="s">
         <v>62</v>
@@ -7156,7 +7318,7 @@
     </row>
     <row r="97" spans="1:21">
       <c r="A97" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B97" t="s">
         <v>72</v>
@@ -7183,7 +7345,7 @@
         <v>52</v>
       </c>
       <c r="J97" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K97" t="s">
         <v>62</v>
@@ -7221,7 +7383,7 @@
     </row>
     <row r="98" spans="1:21">
       <c r="A98" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B98" t="s">
         <v>72</v>
@@ -7248,7 +7410,7 @@
         <v>46</v>
       </c>
       <c r="J98" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K98" t="s">
         <v>62</v>
@@ -7286,7 +7448,7 @@
     </row>
     <row r="99" spans="1:21">
       <c r="A99" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B99" t="s">
         <v>72</v>
@@ -7313,7 +7475,7 @@
         <v>46</v>
       </c>
       <c r="J99" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K99" t="s">
         <v>62</v>
@@ -7351,7 +7513,7 @@
     </row>
     <row r="100" spans="1:21">
       <c r="A100" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B100" t="s">
         <v>72</v>
@@ -7378,7 +7540,7 @@
         <v>46</v>
       </c>
       <c r="J100" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K100" t="s">
         <v>62</v>
@@ -7416,7 +7578,7 @@
     </row>
     <row r="101" spans="1:21">
       <c r="A101" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B101" t="s">
         <v>72</v>
@@ -7443,7 +7605,7 @@
         <v>52</v>
       </c>
       <c r="J101" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K101" t="s">
         <v>62</v>
@@ -7481,7 +7643,7 @@
     </row>
     <row r="102" spans="1:21">
       <c r="A102" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B102" t="s">
         <v>72</v>
@@ -7508,7 +7670,7 @@
         <v>52</v>
       </c>
       <c r="J102" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K102" t="s">
         <v>62</v>
@@ -7546,7 +7708,7 @@
     </row>
     <row r="103" spans="1:21">
       <c r="A103" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B103" t="s">
         <v>72</v>
@@ -7573,7 +7735,7 @@
         <v>52</v>
       </c>
       <c r="J103" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="K103" t="s">
         <v>62</v>
@@ -7609,177 +7771,3492 @@
         <v>50</v>
       </c>
     </row>
-    <row r="104" spans="1:21" s="1" customFormat="1">
-      <c r="A104" s="1" t="s">
+    <row r="104" spans="1:21">
+      <c r="A104" t="s">
+        <v>173</v>
+      </c>
+      <c r="B104" t="s">
+        <v>22</v>
+      </c>
+      <c r="C104" t="s">
+        <v>23</v>
+      </c>
+      <c r="D104" t="s">
+        <v>24</v>
+      </c>
+      <c r="E104" t="s">
+        <v>25</v>
+      </c>
+      <c r="F104" t="s">
+        <v>26</v>
+      </c>
+      <c r="G104" t="s">
+        <v>27</v>
+      </c>
+      <c r="H104" t="s">
+        <v>28</v>
+      </c>
+      <c r="I104" t="s">
+        <v>29</v>
+      </c>
+      <c r="J104" t="s">
+        <v>31</v>
+      </c>
+      <c r="K104" t="s">
+        <v>31</v>
+      </c>
+      <c r="L104" t="s">
+        <v>32</v>
+      </c>
+      <c r="M104" t="s">
+        <v>33</v>
+      </c>
+      <c r="N104" t="s">
+        <v>34</v>
+      </c>
+      <c r="O104" t="s">
+        <v>35</v>
+      </c>
+      <c r="P104" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q104" t="s">
+        <v>36</v>
+      </c>
+      <c r="R104" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S104" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T104" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U104" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="105" spans="1:21">
+      <c r="A105" t="s">
+        <v>174</v>
+      </c>
+      <c r="B105" t="s">
+        <v>39</v>
+      </c>
+      <c r="C105" t="s">
+        <v>40</v>
+      </c>
+      <c r="D105" t="s">
+        <v>41</v>
+      </c>
+      <c r="E105" t="s">
+        <v>42</v>
+      </c>
+      <c r="F105" t="s">
+        <v>43</v>
+      </c>
+      <c r="G105" t="s">
+        <v>44</v>
+      </c>
+      <c r="H105" t="s">
+        <v>45</v>
+      </c>
+      <c r="I105" t="s">
+        <v>46</v>
+      </c>
+      <c r="J105" t="s">
+        <v>48</v>
+      </c>
+      <c r="K105" t="s">
+        <v>48</v>
+      </c>
+      <c r="L105" t="s">
+        <v>32</v>
+      </c>
+      <c r="M105" t="s">
+        <v>33</v>
+      </c>
+      <c r="N105" t="s">
+        <v>34</v>
+      </c>
+      <c r="O105" t="s">
+        <v>35</v>
+      </c>
+      <c r="P105" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q105" t="s">
+        <v>49</v>
+      </c>
+      <c r="R105" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S105" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T105" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U105" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="106" spans="1:21">
+      <c r="A106" t="s">
+        <v>175</v>
+      </c>
+      <c r="B106" t="s">
+        <v>39</v>
+      </c>
+      <c r="C106" t="s">
+        <v>40</v>
+      </c>
+      <c r="D106" t="s">
+        <v>41</v>
+      </c>
+      <c r="E106" t="s">
+        <v>42</v>
+      </c>
+      <c r="F106" t="s">
+        <v>43</v>
+      </c>
+      <c r="G106" t="s">
+        <v>44</v>
+      </c>
+      <c r="H106" t="s">
+        <v>45</v>
+      </c>
+      <c r="I106" t="s">
+        <v>52</v>
+      </c>
+      <c r="J106" t="s">
+        <v>48</v>
+      </c>
+      <c r="K106" t="s">
+        <v>48</v>
+      </c>
+      <c r="L106" t="s">
+        <v>32</v>
+      </c>
+      <c r="M106" t="s">
+        <v>33</v>
+      </c>
+      <c r="N106" t="s">
+        <v>34</v>
+      </c>
+      <c r="O106" t="s">
+        <v>35</v>
+      </c>
+      <c r="P106" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q106" t="s">
+        <v>49</v>
+      </c>
+      <c r="R106" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S106" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T106" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U106" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="107" spans="1:21">
+      <c r="A107" t="s">
+        <v>176</v>
+      </c>
+      <c r="B107" t="s">
+        <v>54</v>
+      </c>
+      <c r="C107" t="s">
+        <v>55</v>
+      </c>
+      <c r="D107" t="s">
+        <v>56</v>
+      </c>
+      <c r="E107" t="s">
+        <v>57</v>
+      </c>
+      <c r="F107" t="s">
+        <v>58</v>
+      </c>
+      <c r="G107" t="s">
+        <v>59</v>
+      </c>
+      <c r="H107" t="s">
+        <v>60</v>
+      </c>
+      <c r="I107" t="s">
+        <v>46</v>
+      </c>
+      <c r="J107" t="s">
+        <v>62</v>
+      </c>
+      <c r="K107" t="s">
+        <v>62</v>
+      </c>
+      <c r="L107" t="s">
+        <v>32</v>
+      </c>
+      <c r="M107" t="s">
+        <v>33</v>
+      </c>
+      <c r="N107" t="s">
+        <v>34</v>
+      </c>
+      <c r="O107" t="s">
+        <v>35</v>
+      </c>
+      <c r="P107" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q107" t="s">
+        <v>63</v>
+      </c>
+      <c r="R107" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S107" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T107" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U107" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="108" spans="1:21">
+      <c r="A108" t="s">
+        <v>177</v>
+      </c>
+      <c r="B108" t="s">
+        <v>54</v>
+      </c>
+      <c r="C108" t="s">
+        <v>55</v>
+      </c>
+      <c r="D108" t="s">
+        <v>56</v>
+      </c>
+      <c r="E108" t="s">
+        <v>57</v>
+      </c>
+      <c r="F108" t="s">
+        <v>58</v>
+      </c>
+      <c r="G108" t="s">
+        <v>59</v>
+      </c>
+      <c r="H108" t="s">
+        <v>60</v>
+      </c>
+      <c r="I108" t="s">
+        <v>52</v>
+      </c>
+      <c r="J108" t="s">
+        <v>62</v>
+      </c>
+      <c r="K108" t="s">
+        <v>62</v>
+      </c>
+      <c r="L108" t="s">
+        <v>32</v>
+      </c>
+      <c r="M108" t="s">
+        <v>33</v>
+      </c>
+      <c r="N108" t="s">
+        <v>34</v>
+      </c>
+      <c r="O108" t="s">
+        <v>35</v>
+      </c>
+      <c r="P108" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q108" t="s">
+        <v>63</v>
+      </c>
+      <c r="R108" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S108" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T108" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U108" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="109" spans="1:21">
+      <c r="A109" t="s">
+        <v>178</v>
+      </c>
+      <c r="B109" t="s">
+        <v>66</v>
+      </c>
+      <c r="C109" t="s">
+        <v>67</v>
+      </c>
+      <c r="D109" t="s">
+        <v>68</v>
+      </c>
+      <c r="E109" t="s">
+        <v>69</v>
+      </c>
+      <c r="F109" t="s">
+        <v>58</v>
+      </c>
+      <c r="G109" t="s">
+        <v>59</v>
+      </c>
+      <c r="H109" t="s">
+        <v>60</v>
+      </c>
+      <c r="I109" t="s">
+        <v>46</v>
+      </c>
+      <c r="J109" t="s">
+        <v>62</v>
+      </c>
+      <c r="K109" t="s">
+        <v>62</v>
+      </c>
+      <c r="L109" t="s">
+        <v>32</v>
+      </c>
+      <c r="M109" t="s">
+        <v>33</v>
+      </c>
+      <c r="N109" t="s">
+        <v>34</v>
+      </c>
+      <c r="O109" t="s">
+        <v>35</v>
+      </c>
+      <c r="P109" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q109" t="s">
+        <v>63</v>
+      </c>
+      <c r="R109" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S109" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T109" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U109" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="110" spans="1:21">
+      <c r="A110" t="s">
+        <v>179</v>
+      </c>
+      <c r="B110" t="s">
+        <v>66</v>
+      </c>
+      <c r="C110" t="s">
+        <v>67</v>
+      </c>
+      <c r="D110" t="s">
+        <v>68</v>
+      </c>
+      <c r="E110" t="s">
+        <v>69</v>
+      </c>
+      <c r="F110" t="s">
+        <v>58</v>
+      </c>
+      <c r="G110" t="s">
+        <v>59</v>
+      </c>
+      <c r="H110" t="s">
+        <v>60</v>
+      </c>
+      <c r="I110" t="s">
+        <v>52</v>
+      </c>
+      <c r="J110" t="s">
+        <v>62</v>
+      </c>
+      <c r="K110" t="s">
+        <v>62</v>
+      </c>
+      <c r="L110" t="s">
+        <v>32</v>
+      </c>
+      <c r="M110" t="s">
+        <v>33</v>
+      </c>
+      <c r="N110" t="s">
+        <v>34</v>
+      </c>
+      <c r="O110" t="s">
+        <v>35</v>
+      </c>
+      <c r="P110" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q110" t="s">
+        <v>63</v>
+      </c>
+      <c r="R110" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S110" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T110" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U110" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="111" spans="1:21">
+      <c r="A111" t="s">
+        <v>180</v>
+      </c>
+      <c r="B111" t="s">
+        <v>72</v>
+      </c>
+      <c r="C111" t="s">
+        <v>73</v>
+      </c>
+      <c r="D111" t="s">
+        <v>74</v>
+      </c>
+      <c r="E111" t="s">
+        <v>75</v>
+      </c>
+      <c r="F111" t="s">
+        <v>58</v>
+      </c>
+      <c r="G111" t="s">
+        <v>59</v>
+      </c>
+      <c r="H111" t="s">
+        <v>60</v>
+      </c>
+      <c r="I111" t="s">
+        <v>46</v>
+      </c>
+      <c r="J111" t="s">
+        <v>62</v>
+      </c>
+      <c r="K111" t="s">
+        <v>62</v>
+      </c>
+      <c r="L111" t="s">
+        <v>32</v>
+      </c>
+      <c r="M111" t="s">
+        <v>33</v>
+      </c>
+      <c r="N111" t="s">
+        <v>34</v>
+      </c>
+      <c r="O111" t="s">
+        <v>35</v>
+      </c>
+      <c r="P111" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q111" t="s">
+        <v>63</v>
+      </c>
+      <c r="R111" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S111" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T111" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U111" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="112" spans="1:21">
+      <c r="A112" t="s">
+        <v>181</v>
+      </c>
+      <c r="B112" t="s">
+        <v>72</v>
+      </c>
+      <c r="C112" t="s">
+        <v>73</v>
+      </c>
+      <c r="D112" t="s">
+        <v>74</v>
+      </c>
+      <c r="E112" t="s">
+        <v>75</v>
+      </c>
+      <c r="F112" t="s">
+        <v>58</v>
+      </c>
+      <c r="G112" t="s">
+        <v>59</v>
+      </c>
+      <c r="H112" t="s">
+        <v>60</v>
+      </c>
+      <c r="I112" t="s">
+        <v>52</v>
+      </c>
+      <c r="J112" t="s">
+        <v>62</v>
+      </c>
+      <c r="K112" t="s">
+        <v>62</v>
+      </c>
+      <c r="L112" t="s">
+        <v>32</v>
+      </c>
+      <c r="M112" t="s">
+        <v>33</v>
+      </c>
+      <c r="N112" t="s">
+        <v>34</v>
+      </c>
+      <c r="O112" t="s">
+        <v>35</v>
+      </c>
+      <c r="P112" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q112" t="s">
+        <v>63</v>
+      </c>
+      <c r="R112" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S112" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T112" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U112" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="113" spans="1:21">
+      <c r="A113" t="s">
+        <v>182</v>
+      </c>
+      <c r="B113" t="s">
+        <v>39</v>
+      </c>
+      <c r="C113" t="s">
+        <v>40</v>
+      </c>
+      <c r="D113" t="s">
+        <v>41</v>
+      </c>
+      <c r="E113" t="s">
+        <v>42</v>
+      </c>
+      <c r="F113" t="s">
+        <v>43</v>
+      </c>
+      <c r="G113" t="s">
+        <v>44</v>
+      </c>
+      <c r="H113" t="s">
+        <v>60</v>
+      </c>
+      <c r="I113" t="s">
+        <v>46</v>
+      </c>
+      <c r="J113" t="s">
+        <v>48</v>
+      </c>
+      <c r="K113" t="s">
+        <v>48</v>
+      </c>
+      <c r="L113" t="s">
+        <v>32</v>
+      </c>
+      <c r="M113" t="s">
+        <v>33</v>
+      </c>
+      <c r="N113" t="s">
+        <v>34</v>
+      </c>
+      <c r="O113" t="s">
+        <v>35</v>
+      </c>
+      <c r="P113" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q113" t="s">
+        <v>49</v>
+      </c>
+      <c r="R113" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S113" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T113" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U113" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="114" spans="1:21">
+      <c r="A114" t="s">
+        <v>183</v>
+      </c>
+      <c r="B114" t="s">
+        <v>39</v>
+      </c>
+      <c r="C114" t="s">
+        <v>40</v>
+      </c>
+      <c r="D114" t="s">
+        <v>41</v>
+      </c>
+      <c r="E114" t="s">
+        <v>42</v>
+      </c>
+      <c r="F114" t="s">
+        <v>43</v>
+      </c>
+      <c r="G114" t="s">
+        <v>59</v>
+      </c>
+      <c r="H114" t="s">
+        <v>45</v>
+      </c>
+      <c r="I114" t="s">
+        <v>46</v>
+      </c>
+      <c r="J114" t="s">
+        <v>48</v>
+      </c>
+      <c r="K114" t="s">
+        <v>48</v>
+      </c>
+      <c r="L114" t="s">
+        <v>32</v>
+      </c>
+      <c r="M114" t="s">
+        <v>33</v>
+      </c>
+      <c r="N114" t="s">
+        <v>34</v>
+      </c>
+      <c r="O114" t="s">
+        <v>35</v>
+      </c>
+      <c r="P114" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q114" t="s">
+        <v>49</v>
+      </c>
+      <c r="R114" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S114" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T114" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U114" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="115" spans="1:21">
+      <c r="A115" t="s">
+        <v>184</v>
+      </c>
+      <c r="B115" t="s">
+        <v>39</v>
+      </c>
+      <c r="C115" t="s">
+        <v>40</v>
+      </c>
+      <c r="D115" t="s">
+        <v>41</v>
+      </c>
+      <c r="E115" t="s">
+        <v>42</v>
+      </c>
+      <c r="F115" t="s">
+        <v>43</v>
+      </c>
+      <c r="G115" t="s">
+        <v>59</v>
+      </c>
+      <c r="H115" t="s">
+        <v>60</v>
+      </c>
+      <c r="I115" t="s">
+        <v>46</v>
+      </c>
+      <c r="J115" t="s">
+        <v>48</v>
+      </c>
+      <c r="K115" t="s">
+        <v>48</v>
+      </c>
+      <c r="L115" t="s">
+        <v>32</v>
+      </c>
+      <c r="M115" t="s">
+        <v>33</v>
+      </c>
+      <c r="N115" t="s">
+        <v>34</v>
+      </c>
+      <c r="O115" t="s">
+        <v>35</v>
+      </c>
+      <c r="P115" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q115" t="s">
+        <v>49</v>
+      </c>
+      <c r="R115" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S115" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T115" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U115" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="116" spans="1:21">
+      <c r="A116" t="s">
+        <v>185</v>
+      </c>
+      <c r="B116" t="s">
+        <v>39</v>
+      </c>
+      <c r="C116" t="s">
+        <v>40</v>
+      </c>
+      <c r="D116" t="s">
+        <v>41</v>
+      </c>
+      <c r="E116" t="s">
+        <v>42</v>
+      </c>
+      <c r="F116" t="s">
+        <v>43</v>
+      </c>
+      <c r="G116" t="s">
+        <v>44</v>
+      </c>
+      <c r="H116" t="s">
+        <v>60</v>
+      </c>
+      <c r="I116" t="s">
+        <v>52</v>
+      </c>
+      <c r="J116" t="s">
+        <v>48</v>
+      </c>
+      <c r="K116" t="s">
+        <v>48</v>
+      </c>
+      <c r="L116" t="s">
+        <v>32</v>
+      </c>
+      <c r="M116" t="s">
+        <v>33</v>
+      </c>
+      <c r="N116" t="s">
+        <v>34</v>
+      </c>
+      <c r="O116" t="s">
+        <v>35</v>
+      </c>
+      <c r="P116" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q116" t="s">
+        <v>49</v>
+      </c>
+      <c r="R116" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S116" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T116" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U116" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="117" spans="1:21">
+      <c r="A117" t="s">
+        <v>186</v>
+      </c>
+      <c r="B117" t="s">
+        <v>39</v>
+      </c>
+      <c r="C117" t="s">
+        <v>40</v>
+      </c>
+      <c r="D117" t="s">
+        <v>41</v>
+      </c>
+      <c r="E117" t="s">
+        <v>42</v>
+      </c>
+      <c r="F117" t="s">
+        <v>43</v>
+      </c>
+      <c r="G117" t="s">
+        <v>59</v>
+      </c>
+      <c r="H117" t="s">
+        <v>45</v>
+      </c>
+      <c r="I117" t="s">
+        <v>52</v>
+      </c>
+      <c r="J117" t="s">
+        <v>48</v>
+      </c>
+      <c r="K117" t="s">
+        <v>48</v>
+      </c>
+      <c r="L117" t="s">
+        <v>32</v>
+      </c>
+      <c r="M117" t="s">
+        <v>33</v>
+      </c>
+      <c r="N117" t="s">
+        <v>34</v>
+      </c>
+      <c r="O117" t="s">
+        <v>35</v>
+      </c>
+      <c r="P117" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q117" t="s">
+        <v>49</v>
+      </c>
+      <c r="R117" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S117" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T117" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U117" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="118" spans="1:21">
+      <c r="A118" t="s">
+        <v>187</v>
+      </c>
+      <c r="B118" t="s">
+        <v>39</v>
+      </c>
+      <c r="C118" t="s">
+        <v>40</v>
+      </c>
+      <c r="D118" t="s">
+        <v>41</v>
+      </c>
+      <c r="E118" t="s">
+        <v>42</v>
+      </c>
+      <c r="F118" t="s">
+        <v>43</v>
+      </c>
+      <c r="G118" t="s">
+        <v>59</v>
+      </c>
+      <c r="H118" t="s">
+        <v>60</v>
+      </c>
+      <c r="I118" t="s">
+        <v>52</v>
+      </c>
+      <c r="J118" t="s">
+        <v>48</v>
+      </c>
+      <c r="K118" t="s">
+        <v>48</v>
+      </c>
+      <c r="L118" t="s">
+        <v>32</v>
+      </c>
+      <c r="M118" t="s">
+        <v>33</v>
+      </c>
+      <c r="N118" t="s">
+        <v>34</v>
+      </c>
+      <c r="O118" t="s">
+        <v>35</v>
+      </c>
+      <c r="P118" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q118" t="s">
+        <v>49</v>
+      </c>
+      <c r="R118" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S118" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T118" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U118" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="119" spans="1:21">
+      <c r="A119" t="s">
+        <v>188</v>
+      </c>
+      <c r="B119" t="s">
+        <v>54</v>
+      </c>
+      <c r="C119" t="s">
+        <v>55</v>
+      </c>
+      <c r="D119" t="s">
+        <v>56</v>
+      </c>
+      <c r="E119" t="s">
+        <v>57</v>
+      </c>
+      <c r="F119" t="s">
+        <v>58</v>
+      </c>
+      <c r="G119" t="s">
+        <v>44</v>
+      </c>
+      <c r="H119" t="s">
+        <v>45</v>
+      </c>
+      <c r="I119" t="s">
+        <v>46</v>
+      </c>
+      <c r="J119" t="s">
+        <v>62</v>
+      </c>
+      <c r="K119" t="s">
+        <v>62</v>
+      </c>
+      <c r="L119" t="s">
+        <v>32</v>
+      </c>
+      <c r="M119" t="s">
+        <v>33</v>
+      </c>
+      <c r="N119" t="s">
+        <v>34</v>
+      </c>
+      <c r="O119" t="s">
+        <v>35</v>
+      </c>
+      <c r="P119" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q119" t="s">
+        <v>63</v>
+      </c>
+      <c r="R119" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S119" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T119" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U119" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="120" spans="1:21">
+      <c r="A120" t="s">
+        <v>189</v>
+      </c>
+      <c r="B120" t="s">
+        <v>54</v>
+      </c>
+      <c r="C120" t="s">
+        <v>55</v>
+      </c>
+      <c r="D120" t="s">
+        <v>56</v>
+      </c>
+      <c r="E120" t="s">
+        <v>57</v>
+      </c>
+      <c r="F120" t="s">
+        <v>58</v>
+      </c>
+      <c r="G120" t="s">
+        <v>44</v>
+      </c>
+      <c r="H120" t="s">
+        <v>60</v>
+      </c>
+      <c r="I120" t="s">
+        <v>46</v>
+      </c>
+      <c r="J120" t="s">
+        <v>62</v>
+      </c>
+      <c r="K120" t="s">
+        <v>62</v>
+      </c>
+      <c r="L120" t="s">
+        <v>32</v>
+      </c>
+      <c r="M120" t="s">
+        <v>33</v>
+      </c>
+      <c r="N120" t="s">
+        <v>34</v>
+      </c>
+      <c r="O120" t="s">
+        <v>35</v>
+      </c>
+      <c r="P120" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q120" t="s">
+        <v>63</v>
+      </c>
+      <c r="R120" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S120" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T120" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U120" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="121" spans="1:21">
+      <c r="A121" t="s">
+        <v>190</v>
+      </c>
+      <c r="B121" t="s">
+        <v>54</v>
+      </c>
+      <c r="C121" t="s">
+        <v>55</v>
+      </c>
+      <c r="D121" t="s">
+        <v>56</v>
+      </c>
+      <c r="E121" t="s">
+        <v>57</v>
+      </c>
+      <c r="F121" t="s">
+        <v>58</v>
+      </c>
+      <c r="G121" t="s">
+        <v>59</v>
+      </c>
+      <c r="H121" t="s">
+        <v>45</v>
+      </c>
+      <c r="I121" t="s">
+        <v>46</v>
+      </c>
+      <c r="J121" t="s">
+        <v>62</v>
+      </c>
+      <c r="K121" t="s">
+        <v>62</v>
+      </c>
+      <c r="L121" t="s">
+        <v>32</v>
+      </c>
+      <c r="M121" t="s">
+        <v>33</v>
+      </c>
+      <c r="N121" t="s">
+        <v>34</v>
+      </c>
+      <c r="O121" t="s">
+        <v>35</v>
+      </c>
+      <c r="P121" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q121" t="s">
+        <v>63</v>
+      </c>
+      <c r="R121" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S121" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T121" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U121" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="122" spans="1:21">
+      <c r="A122" t="s">
+        <v>191</v>
+      </c>
+      <c r="B122" t="s">
+        <v>54</v>
+      </c>
+      <c r="C122" t="s">
+        <v>55</v>
+      </c>
+      <c r="D122" t="s">
+        <v>56</v>
+      </c>
+      <c r="E122" t="s">
+        <v>57</v>
+      </c>
+      <c r="F122" t="s">
+        <v>58</v>
+      </c>
+      <c r="G122" t="s">
+        <v>44</v>
+      </c>
+      <c r="H122" t="s">
+        <v>45</v>
+      </c>
+      <c r="I122" t="s">
+        <v>52</v>
+      </c>
+      <c r="J122" t="s">
+        <v>62</v>
+      </c>
+      <c r="K122" t="s">
+        <v>62</v>
+      </c>
+      <c r="L122" t="s">
+        <v>32</v>
+      </c>
+      <c r="M122" t="s">
+        <v>33</v>
+      </c>
+      <c r="N122" t="s">
+        <v>34</v>
+      </c>
+      <c r="O122" t="s">
+        <v>35</v>
+      </c>
+      <c r="P122" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q122" t="s">
+        <v>63</v>
+      </c>
+      <c r="R122" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S122" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T122" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U122" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="123" spans="1:21">
+      <c r="A123" t="s">
+        <v>192</v>
+      </c>
+      <c r="B123" t="s">
+        <v>54</v>
+      </c>
+      <c r="C123" t="s">
+        <v>55</v>
+      </c>
+      <c r="D123" t="s">
+        <v>56</v>
+      </c>
+      <c r="E123" t="s">
+        <v>57</v>
+      </c>
+      <c r="F123" t="s">
+        <v>58</v>
+      </c>
+      <c r="G123" t="s">
+        <v>44</v>
+      </c>
+      <c r="H123" t="s">
+        <v>60</v>
+      </c>
+      <c r="I123" t="s">
+        <v>52</v>
+      </c>
+      <c r="J123" t="s">
+        <v>62</v>
+      </c>
+      <c r="K123" t="s">
+        <v>62</v>
+      </c>
+      <c r="L123" t="s">
+        <v>32</v>
+      </c>
+      <c r="M123" t="s">
+        <v>33</v>
+      </c>
+      <c r="N123" t="s">
+        <v>34</v>
+      </c>
+      <c r="O123" t="s">
+        <v>35</v>
+      </c>
+      <c r="P123" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q123" t="s">
+        <v>63</v>
+      </c>
+      <c r="R123" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S123" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T123" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U123" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="124" spans="1:21">
+      <c r="A124" t="s">
+        <v>193</v>
+      </c>
+      <c r="B124" t="s">
+        <v>54</v>
+      </c>
+      <c r="C124" t="s">
+        <v>55</v>
+      </c>
+      <c r="D124" t="s">
+        <v>56</v>
+      </c>
+      <c r="E124" t="s">
+        <v>57</v>
+      </c>
+      <c r="F124" t="s">
+        <v>58</v>
+      </c>
+      <c r="G124" t="s">
+        <v>59</v>
+      </c>
+      <c r="H124" t="s">
+        <v>45</v>
+      </c>
+      <c r="I124" t="s">
+        <v>52</v>
+      </c>
+      <c r="J124" t="s">
+        <v>62</v>
+      </c>
+      <c r="K124" t="s">
+        <v>62</v>
+      </c>
+      <c r="L124" t="s">
+        <v>32</v>
+      </c>
+      <c r="M124" t="s">
+        <v>33</v>
+      </c>
+      <c r="N124" t="s">
+        <v>34</v>
+      </c>
+      <c r="O124" t="s">
+        <v>35</v>
+      </c>
+      <c r="P124" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q124" t="s">
+        <v>63</v>
+      </c>
+      <c r="R124" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S124" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T124" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U124" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="125" spans="1:21">
+      <c r="A125" t="s">
+        <v>194</v>
+      </c>
+      <c r="B125" t="s">
+        <v>54</v>
+      </c>
+      <c r="C125" t="s">
+        <v>55</v>
+      </c>
+      <c r="D125" t="s">
+        <v>56</v>
+      </c>
+      <c r="E125" t="s">
+        <v>57</v>
+      </c>
+      <c r="F125" t="s">
+        <v>58</v>
+      </c>
+      <c r="G125" t="s">
+        <v>44</v>
+      </c>
+      <c r="H125" t="s">
+        <v>45</v>
+      </c>
+      <c r="I125" t="s">
+        <v>46</v>
+      </c>
+      <c r="J125" t="s">
+        <v>62</v>
+      </c>
+      <c r="K125" t="s">
+        <v>62</v>
+      </c>
+      <c r="L125" t="s">
+        <v>32</v>
+      </c>
+      <c r="M125" t="s">
+        <v>33</v>
+      </c>
+      <c r="N125" t="s">
+        <v>34</v>
+      </c>
+      <c r="O125" t="s">
+        <v>35</v>
+      </c>
+      <c r="P125" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q125" t="s">
+        <v>49</v>
+      </c>
+      <c r="R125" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S125" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T125" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U125" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="126" spans="1:21">
+      <c r="A126" t="s">
+        <v>195</v>
+      </c>
+      <c r="B126" t="s">
+        <v>54</v>
+      </c>
+      <c r="C126" t="s">
+        <v>55</v>
+      </c>
+      <c r="D126" t="s">
+        <v>56</v>
+      </c>
+      <c r="E126" t="s">
+        <v>57</v>
+      </c>
+      <c r="F126" t="s">
+        <v>58</v>
+      </c>
+      <c r="G126" t="s">
+        <v>44</v>
+      </c>
+      <c r="H126" t="s">
+        <v>60</v>
+      </c>
+      <c r="I126" t="s">
+        <v>46</v>
+      </c>
+      <c r="J126" t="s">
+        <v>62</v>
+      </c>
+      <c r="K126" t="s">
+        <v>62</v>
+      </c>
+      <c r="L126" t="s">
+        <v>32</v>
+      </c>
+      <c r="M126" t="s">
+        <v>33</v>
+      </c>
+      <c r="N126" t="s">
+        <v>34</v>
+      </c>
+      <c r="O126" t="s">
+        <v>35</v>
+      </c>
+      <c r="P126" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q126" t="s">
+        <v>49</v>
+      </c>
+      <c r="R126" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S126" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T126" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U126" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="127" spans="1:21">
+      <c r="A127" t="s">
+        <v>196</v>
+      </c>
+      <c r="B127" t="s">
+        <v>54</v>
+      </c>
+      <c r="C127" t="s">
+        <v>55</v>
+      </c>
+      <c r="D127" t="s">
+        <v>56</v>
+      </c>
+      <c r="E127" t="s">
+        <v>57</v>
+      </c>
+      <c r="F127" t="s">
+        <v>58</v>
+      </c>
+      <c r="G127" t="s">
+        <v>59</v>
+      </c>
+      <c r="H127" t="s">
+        <v>45</v>
+      </c>
+      <c r="I127" t="s">
+        <v>46</v>
+      </c>
+      <c r="J127" t="s">
+        <v>62</v>
+      </c>
+      <c r="K127" t="s">
+        <v>62</v>
+      </c>
+      <c r="L127" t="s">
+        <v>32</v>
+      </c>
+      <c r="M127" t="s">
+        <v>33</v>
+      </c>
+      <c r="N127" t="s">
+        <v>34</v>
+      </c>
+      <c r="O127" t="s">
+        <v>35</v>
+      </c>
+      <c r="P127" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q127" t="s">
+        <v>49</v>
+      </c>
+      <c r="R127" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S127" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T127" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U127" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="128" spans="1:21">
+      <c r="A128" t="s">
+        <v>197</v>
+      </c>
+      <c r="B128" t="s">
+        <v>54</v>
+      </c>
+      <c r="C128" t="s">
+        <v>55</v>
+      </c>
+      <c r="D128" t="s">
+        <v>56</v>
+      </c>
+      <c r="E128" t="s">
+        <v>57</v>
+      </c>
+      <c r="F128" t="s">
+        <v>58</v>
+      </c>
+      <c r="G128" t="s">
+        <v>44</v>
+      </c>
+      <c r="H128" t="s">
+        <v>45</v>
+      </c>
+      <c r="I128" t="s">
+        <v>52</v>
+      </c>
+      <c r="J128" t="s">
+        <v>62</v>
+      </c>
+      <c r="K128" t="s">
+        <v>62</v>
+      </c>
+      <c r="L128" t="s">
+        <v>32</v>
+      </c>
+      <c r="M128" t="s">
+        <v>33</v>
+      </c>
+      <c r="N128" t="s">
+        <v>34</v>
+      </c>
+      <c r="O128" t="s">
+        <v>35</v>
+      </c>
+      <c r="P128" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q128" t="s">
+        <v>49</v>
+      </c>
+      <c r="R128" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S128" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T128" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U128" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="129" spans="1:21">
+      <c r="A129" t="s">
+        <v>198</v>
+      </c>
+      <c r="B129" t="s">
+        <v>54</v>
+      </c>
+      <c r="C129" t="s">
+        <v>55</v>
+      </c>
+      <c r="D129" t="s">
+        <v>56</v>
+      </c>
+      <c r="E129" t="s">
+        <v>57</v>
+      </c>
+      <c r="F129" t="s">
+        <v>58</v>
+      </c>
+      <c r="G129" t="s">
+        <v>44</v>
+      </c>
+      <c r="H129" t="s">
+        <v>60</v>
+      </c>
+      <c r="I129" t="s">
+        <v>52</v>
+      </c>
+      <c r="J129" t="s">
+        <v>62</v>
+      </c>
+      <c r="K129" t="s">
+        <v>62</v>
+      </c>
+      <c r="L129" t="s">
+        <v>32</v>
+      </c>
+      <c r="M129" t="s">
+        <v>33</v>
+      </c>
+      <c r="N129" t="s">
+        <v>34</v>
+      </c>
+      <c r="O129" t="s">
+        <v>35</v>
+      </c>
+      <c r="P129" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q129" t="s">
+        <v>49</v>
+      </c>
+      <c r="R129" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S129" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T129" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U129" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="130" spans="1:21">
+      <c r="A130" t="s">
+        <v>199</v>
+      </c>
+      <c r="B130" t="s">
+        <v>54</v>
+      </c>
+      <c r="C130" t="s">
+        <v>55</v>
+      </c>
+      <c r="D130" t="s">
+        <v>56</v>
+      </c>
+      <c r="E130" t="s">
+        <v>57</v>
+      </c>
+      <c r="F130" t="s">
+        <v>58</v>
+      </c>
+      <c r="G130" t="s">
+        <v>59</v>
+      </c>
+      <c r="H130" t="s">
+        <v>45</v>
+      </c>
+      <c r="I130" t="s">
+        <v>52</v>
+      </c>
+      <c r="J130" t="s">
+        <v>62</v>
+      </c>
+      <c r="K130" t="s">
+        <v>62</v>
+      </c>
+      <c r="L130" t="s">
+        <v>32</v>
+      </c>
+      <c r="M130" t="s">
+        <v>33</v>
+      </c>
+      <c r="N130" t="s">
+        <v>34</v>
+      </c>
+      <c r="O130" t="s">
+        <v>35</v>
+      </c>
+      <c r="P130" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q130" t="s">
+        <v>49</v>
+      </c>
+      <c r="R130" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S130" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T130" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U130" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="131" spans="1:21">
+      <c r="A131" t="s">
+        <v>200</v>
+      </c>
+      <c r="B131" t="s">
+        <v>66</v>
+      </c>
+      <c r="C131" t="s">
+        <v>67</v>
+      </c>
+      <c r="D131" t="s">
+        <v>68</v>
+      </c>
+      <c r="E131" t="s">
+        <v>69</v>
+      </c>
+      <c r="F131" t="s">
+        <v>58</v>
+      </c>
+      <c r="G131" t="s">
+        <v>44</v>
+      </c>
+      <c r="H131" t="s">
+        <v>45</v>
+      </c>
+      <c r="I131" t="s">
+        <v>46</v>
+      </c>
+      <c r="J131" t="s">
+        <v>62</v>
+      </c>
+      <c r="K131" t="s">
+        <v>62</v>
+      </c>
+      <c r="L131" t="s">
+        <v>32</v>
+      </c>
+      <c r="M131" t="s">
+        <v>33</v>
+      </c>
+      <c r="N131" t="s">
+        <v>34</v>
+      </c>
+      <c r="O131" t="s">
+        <v>35</v>
+      </c>
+      <c r="P131" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q131" t="s">
+        <v>63</v>
+      </c>
+      <c r="R131" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S131" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T131" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U131" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="132" spans="1:21">
+      <c r="A132" t="s">
+        <v>201</v>
+      </c>
+      <c r="B132" t="s">
+        <v>66</v>
+      </c>
+      <c r="C132" t="s">
+        <v>67</v>
+      </c>
+      <c r="D132" t="s">
+        <v>68</v>
+      </c>
+      <c r="E132" t="s">
+        <v>69</v>
+      </c>
+      <c r="F132" t="s">
+        <v>58</v>
+      </c>
+      <c r="G132" t="s">
+        <v>44</v>
+      </c>
+      <c r="H132" t="s">
+        <v>60</v>
+      </c>
+      <c r="I132" t="s">
+        <v>46</v>
+      </c>
+      <c r="J132" t="s">
+        <v>62</v>
+      </c>
+      <c r="K132" t="s">
+        <v>62</v>
+      </c>
+      <c r="L132" t="s">
+        <v>32</v>
+      </c>
+      <c r="M132" t="s">
+        <v>33</v>
+      </c>
+      <c r="N132" t="s">
+        <v>34</v>
+      </c>
+      <c r="O132" t="s">
+        <v>35</v>
+      </c>
+      <c r="P132" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q132" t="s">
+        <v>63</v>
+      </c>
+      <c r="R132" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S132" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T132" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U132" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="133" spans="1:21">
+      <c r="A133" t="s">
+        <v>202</v>
+      </c>
+      <c r="B133" t="s">
+        <v>66</v>
+      </c>
+      <c r="C133" t="s">
+        <v>67</v>
+      </c>
+      <c r="D133" t="s">
+        <v>68</v>
+      </c>
+      <c r="E133" t="s">
+        <v>69</v>
+      </c>
+      <c r="F133" t="s">
+        <v>58</v>
+      </c>
+      <c r="G133" t="s">
+        <v>59</v>
+      </c>
+      <c r="H133" t="s">
+        <v>45</v>
+      </c>
+      <c r="I133" t="s">
+        <v>46</v>
+      </c>
+      <c r="J133" t="s">
+        <v>62</v>
+      </c>
+      <c r="K133" t="s">
+        <v>62</v>
+      </c>
+      <c r="L133" t="s">
+        <v>32</v>
+      </c>
+      <c r="M133" t="s">
+        <v>33</v>
+      </c>
+      <c r="N133" t="s">
+        <v>34</v>
+      </c>
+      <c r="O133" t="s">
+        <v>35</v>
+      </c>
+      <c r="P133" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q133" t="s">
+        <v>63</v>
+      </c>
+      <c r="R133" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S133" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T133" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U133" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="134" spans="1:21">
+      <c r="A134" t="s">
+        <v>203</v>
+      </c>
+      <c r="B134" t="s">
+        <v>66</v>
+      </c>
+      <c r="C134" t="s">
+        <v>67</v>
+      </c>
+      <c r="D134" t="s">
+        <v>68</v>
+      </c>
+      <c r="E134" t="s">
+        <v>69</v>
+      </c>
+      <c r="F134" t="s">
+        <v>58</v>
+      </c>
+      <c r="G134" t="s">
+        <v>44</v>
+      </c>
+      <c r="H134" t="s">
+        <v>45</v>
+      </c>
+      <c r="I134" t="s">
+        <v>52</v>
+      </c>
+      <c r="J134" t="s">
+        <v>62</v>
+      </c>
+      <c r="K134" t="s">
+        <v>62</v>
+      </c>
+      <c r="L134" t="s">
+        <v>32</v>
+      </c>
+      <c r="M134" t="s">
+        <v>33</v>
+      </c>
+      <c r="N134" t="s">
+        <v>34</v>
+      </c>
+      <c r="O134" t="s">
+        <v>35</v>
+      </c>
+      <c r="P134" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q134" t="s">
+        <v>63</v>
+      </c>
+      <c r="R134" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S134" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T134" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U134" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="135" spans="1:21">
+      <c r="A135" t="s">
+        <v>204</v>
+      </c>
+      <c r="B135" t="s">
+        <v>66</v>
+      </c>
+      <c r="C135" t="s">
+        <v>67</v>
+      </c>
+      <c r="D135" t="s">
+        <v>68</v>
+      </c>
+      <c r="E135" t="s">
+        <v>69</v>
+      </c>
+      <c r="F135" t="s">
+        <v>58</v>
+      </c>
+      <c r="G135" t="s">
+        <v>44</v>
+      </c>
+      <c r="H135" t="s">
+        <v>60</v>
+      </c>
+      <c r="I135" t="s">
+        <v>52</v>
+      </c>
+      <c r="J135" t="s">
+        <v>62</v>
+      </c>
+      <c r="K135" t="s">
+        <v>62</v>
+      </c>
+      <c r="L135" t="s">
+        <v>32</v>
+      </c>
+      <c r="M135" t="s">
+        <v>33</v>
+      </c>
+      <c r="N135" t="s">
+        <v>34</v>
+      </c>
+      <c r="O135" t="s">
+        <v>35</v>
+      </c>
+      <c r="P135" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q135" t="s">
+        <v>63</v>
+      </c>
+      <c r="R135" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S135" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T135" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U135" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="136" spans="1:21">
+      <c r="A136" t="s">
+        <v>205</v>
+      </c>
+      <c r="B136" t="s">
+        <v>66</v>
+      </c>
+      <c r="C136" t="s">
+        <v>67</v>
+      </c>
+      <c r="D136" t="s">
+        <v>68</v>
+      </c>
+      <c r="E136" t="s">
+        <v>69</v>
+      </c>
+      <c r="F136" t="s">
+        <v>58</v>
+      </c>
+      <c r="G136" t="s">
+        <v>59</v>
+      </c>
+      <c r="H136" t="s">
+        <v>45</v>
+      </c>
+      <c r="I136" t="s">
+        <v>52</v>
+      </c>
+      <c r="J136" t="s">
+        <v>62</v>
+      </c>
+      <c r="K136" t="s">
+        <v>62</v>
+      </c>
+      <c r="L136" t="s">
+        <v>32</v>
+      </c>
+      <c r="M136" t="s">
+        <v>33</v>
+      </c>
+      <c r="N136" t="s">
+        <v>34</v>
+      </c>
+      <c r="O136" t="s">
+        <v>35</v>
+      </c>
+      <c r="P136" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q136" t="s">
+        <v>63</v>
+      </c>
+      <c r="R136" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S136" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T136" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U136" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="137" spans="1:21">
+      <c r="A137" t="s">
+        <v>206</v>
+      </c>
+      <c r="B137" t="s">
+        <v>66</v>
+      </c>
+      <c r="C137" t="s">
+        <v>67</v>
+      </c>
+      <c r="D137" t="s">
+        <v>68</v>
+      </c>
+      <c r="E137" t="s">
+        <v>69</v>
+      </c>
+      <c r="F137" t="s">
+        <v>58</v>
+      </c>
+      <c r="G137" t="s">
+        <v>44</v>
+      </c>
+      <c r="H137" t="s">
+        <v>45</v>
+      </c>
+      <c r="I137" t="s">
+        <v>46</v>
+      </c>
+      <c r="J137" t="s">
+        <v>62</v>
+      </c>
+      <c r="K137" t="s">
+        <v>62</v>
+      </c>
+      <c r="L137" t="s">
+        <v>32</v>
+      </c>
+      <c r="M137" t="s">
+        <v>33</v>
+      </c>
+      <c r="N137" t="s">
+        <v>34</v>
+      </c>
+      <c r="O137" t="s">
+        <v>35</v>
+      </c>
+      <c r="P137" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q137" t="s">
+        <v>49</v>
+      </c>
+      <c r="R137" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S137" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T137" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U137" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="138" spans="1:21">
+      <c r="A138" t="s">
+        <v>207</v>
+      </c>
+      <c r="B138" t="s">
+        <v>66</v>
+      </c>
+      <c r="C138" t="s">
+        <v>67</v>
+      </c>
+      <c r="D138" t="s">
+        <v>68</v>
+      </c>
+      <c r="E138" t="s">
+        <v>69</v>
+      </c>
+      <c r="F138" t="s">
+        <v>58</v>
+      </c>
+      <c r="G138" t="s">
+        <v>44</v>
+      </c>
+      <c r="H138" t="s">
+        <v>60</v>
+      </c>
+      <c r="I138" t="s">
+        <v>46</v>
+      </c>
+      <c r="J138" t="s">
+        <v>62</v>
+      </c>
+      <c r="K138" t="s">
+        <v>62</v>
+      </c>
+      <c r="L138" t="s">
+        <v>32</v>
+      </c>
+      <c r="M138" t="s">
+        <v>33</v>
+      </c>
+      <c r="N138" t="s">
+        <v>34</v>
+      </c>
+      <c r="O138" t="s">
+        <v>35</v>
+      </c>
+      <c r="P138" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q138" t="s">
+        <v>49</v>
+      </c>
+      <c r="R138" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S138" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T138" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U138" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="139" spans="1:21">
+      <c r="A139" t="s">
+        <v>208</v>
+      </c>
+      <c r="B139" t="s">
+        <v>66</v>
+      </c>
+      <c r="C139" t="s">
+        <v>67</v>
+      </c>
+      <c r="D139" t="s">
+        <v>68</v>
+      </c>
+      <c r="E139" t="s">
+        <v>69</v>
+      </c>
+      <c r="F139" t="s">
+        <v>58</v>
+      </c>
+      <c r="G139" t="s">
+        <v>59</v>
+      </c>
+      <c r="H139" t="s">
+        <v>45</v>
+      </c>
+      <c r="I139" t="s">
+        <v>46</v>
+      </c>
+      <c r="J139" t="s">
+        <v>62</v>
+      </c>
+      <c r="K139" t="s">
+        <v>62</v>
+      </c>
+      <c r="L139" t="s">
+        <v>32</v>
+      </c>
+      <c r="M139" t="s">
+        <v>33</v>
+      </c>
+      <c r="N139" t="s">
+        <v>34</v>
+      </c>
+      <c r="O139" t="s">
+        <v>35</v>
+      </c>
+      <c r="P139" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q139" t="s">
+        <v>49</v>
+      </c>
+      <c r="R139" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S139" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T139" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U139" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="140" spans="1:21">
+      <c r="A140" t="s">
+        <v>209</v>
+      </c>
+      <c r="B140" t="s">
+        <v>66</v>
+      </c>
+      <c r="C140" t="s">
+        <v>67</v>
+      </c>
+      <c r="D140" t="s">
+        <v>68</v>
+      </c>
+      <c r="E140" t="s">
+        <v>69</v>
+      </c>
+      <c r="F140" t="s">
+        <v>58</v>
+      </c>
+      <c r="G140" t="s">
+        <v>44</v>
+      </c>
+      <c r="H140" t="s">
+        <v>45</v>
+      </c>
+      <c r="I140" t="s">
+        <v>52</v>
+      </c>
+      <c r="J140" t="s">
+        <v>62</v>
+      </c>
+      <c r="K140" t="s">
+        <v>62</v>
+      </c>
+      <c r="L140" t="s">
+        <v>32</v>
+      </c>
+      <c r="M140" t="s">
+        <v>33</v>
+      </c>
+      <c r="N140" t="s">
+        <v>34</v>
+      </c>
+      <c r="O140" t="s">
+        <v>35</v>
+      </c>
+      <c r="P140" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q140" t="s">
+        <v>49</v>
+      </c>
+      <c r="R140" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S140" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T140" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U140" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="141" spans="1:21">
+      <c r="A141" t="s">
+        <v>210</v>
+      </c>
+      <c r="B141" t="s">
+        <v>66</v>
+      </c>
+      <c r="C141" t="s">
+        <v>67</v>
+      </c>
+      <c r="D141" t="s">
+        <v>68</v>
+      </c>
+      <c r="E141" t="s">
+        <v>69</v>
+      </c>
+      <c r="F141" t="s">
+        <v>58</v>
+      </c>
+      <c r="G141" t="s">
+        <v>44</v>
+      </c>
+      <c r="H141" t="s">
+        <v>60</v>
+      </c>
+      <c r="I141" t="s">
+        <v>52</v>
+      </c>
+      <c r="J141" t="s">
+        <v>62</v>
+      </c>
+      <c r="K141" t="s">
+        <v>62</v>
+      </c>
+      <c r="L141" t="s">
+        <v>32</v>
+      </c>
+      <c r="M141" t="s">
+        <v>33</v>
+      </c>
+      <c r="N141" t="s">
+        <v>34</v>
+      </c>
+      <c r="O141" t="s">
+        <v>35</v>
+      </c>
+      <c r="P141" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q141" t="s">
+        <v>49</v>
+      </c>
+      <c r="R141" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S141" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T141" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U141" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="142" spans="1:21">
+      <c r="A142" t="s">
+        <v>211</v>
+      </c>
+      <c r="B142" t="s">
+        <v>66</v>
+      </c>
+      <c r="C142" t="s">
+        <v>67</v>
+      </c>
+      <c r="D142" t="s">
+        <v>68</v>
+      </c>
+      <c r="E142" t="s">
+        <v>69</v>
+      </c>
+      <c r="F142" t="s">
+        <v>58</v>
+      </c>
+      <c r="G142" t="s">
+        <v>59</v>
+      </c>
+      <c r="H142" t="s">
+        <v>45</v>
+      </c>
+      <c r="I142" t="s">
+        <v>52</v>
+      </c>
+      <c r="J142" t="s">
+        <v>62</v>
+      </c>
+      <c r="K142" t="s">
+        <v>62</v>
+      </c>
+      <c r="L142" t="s">
+        <v>32</v>
+      </c>
+      <c r="M142" t="s">
+        <v>33</v>
+      </c>
+      <c r="N142" t="s">
+        <v>34</v>
+      </c>
+      <c r="O142" t="s">
+        <v>35</v>
+      </c>
+      <c r="P142" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q142" t="s">
+        <v>49</v>
+      </c>
+      <c r="R142" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S142" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T142" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U142" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="143" spans="1:21">
+      <c r="A143" t="s">
+        <v>212</v>
+      </c>
+      <c r="B143" t="s">
+        <v>72</v>
+      </c>
+      <c r="C143" t="s">
+        <v>73</v>
+      </c>
+      <c r="D143" t="s">
+        <v>74</v>
+      </c>
+      <c r="E143" t="s">
+        <v>75</v>
+      </c>
+      <c r="F143" t="s">
+        <v>58</v>
+      </c>
+      <c r="G143" t="s">
+        <v>44</v>
+      </c>
+      <c r="H143" t="s">
+        <v>45</v>
+      </c>
+      <c r="I143" t="s">
+        <v>46</v>
+      </c>
+      <c r="J143" t="s">
+        <v>62</v>
+      </c>
+      <c r="K143" t="s">
+        <v>62</v>
+      </c>
+      <c r="L143" t="s">
+        <v>32</v>
+      </c>
+      <c r="M143" t="s">
+        <v>33</v>
+      </c>
+      <c r="N143" t="s">
+        <v>34</v>
+      </c>
+      <c r="O143" t="s">
+        <v>35</v>
+      </c>
+      <c r="P143" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q143" t="s">
+        <v>63</v>
+      </c>
+      <c r="R143" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S143" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T143" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U143" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="144" spans="1:21">
+      <c r="A144" t="s">
+        <v>213</v>
+      </c>
+      <c r="B144" t="s">
+        <v>72</v>
+      </c>
+      <c r="C144" t="s">
+        <v>73</v>
+      </c>
+      <c r="D144" t="s">
+        <v>74</v>
+      </c>
+      <c r="E144" t="s">
+        <v>75</v>
+      </c>
+      <c r="F144" t="s">
+        <v>58</v>
+      </c>
+      <c r="G144" t="s">
+        <v>44</v>
+      </c>
+      <c r="H144" t="s">
+        <v>60</v>
+      </c>
+      <c r="I144" t="s">
+        <v>46</v>
+      </c>
+      <c r="J144" t="s">
+        <v>62</v>
+      </c>
+      <c r="K144" t="s">
+        <v>62</v>
+      </c>
+      <c r="L144" t="s">
+        <v>32</v>
+      </c>
+      <c r="M144" t="s">
+        <v>33</v>
+      </c>
+      <c r="N144" t="s">
+        <v>34</v>
+      </c>
+      <c r="O144" t="s">
+        <v>35</v>
+      </c>
+      <c r="P144" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q144" t="s">
+        <v>63</v>
+      </c>
+      <c r="R144" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S144" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T144" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U144" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="145" spans="1:21">
+      <c r="A145" t="s">
+        <v>214</v>
+      </c>
+      <c r="B145" t="s">
+        <v>72</v>
+      </c>
+      <c r="C145" t="s">
+        <v>73</v>
+      </c>
+      <c r="D145" t="s">
+        <v>74</v>
+      </c>
+      <c r="E145" t="s">
+        <v>75</v>
+      </c>
+      <c r="F145" t="s">
+        <v>58</v>
+      </c>
+      <c r="G145" t="s">
+        <v>59</v>
+      </c>
+      <c r="H145" t="s">
+        <v>45</v>
+      </c>
+      <c r="I145" t="s">
+        <v>46</v>
+      </c>
+      <c r="J145" t="s">
+        <v>62</v>
+      </c>
+      <c r="K145" t="s">
+        <v>62</v>
+      </c>
+      <c r="L145" t="s">
+        <v>32</v>
+      </c>
+      <c r="M145" t="s">
+        <v>33</v>
+      </c>
+      <c r="N145" t="s">
+        <v>34</v>
+      </c>
+      <c r="O145" t="s">
+        <v>35</v>
+      </c>
+      <c r="P145" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q145" t="s">
+        <v>63</v>
+      </c>
+      <c r="R145" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S145" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T145" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U145" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="146" spans="1:21">
+      <c r="A146" t="s">
+        <v>215</v>
+      </c>
+      <c r="B146" t="s">
+        <v>72</v>
+      </c>
+      <c r="C146" t="s">
+        <v>73</v>
+      </c>
+      <c r="D146" t="s">
+        <v>74</v>
+      </c>
+      <c r="E146" t="s">
+        <v>75</v>
+      </c>
+      <c r="F146" t="s">
+        <v>58</v>
+      </c>
+      <c r="G146" t="s">
+        <v>44</v>
+      </c>
+      <c r="H146" t="s">
+        <v>45</v>
+      </c>
+      <c r="I146" t="s">
+        <v>52</v>
+      </c>
+      <c r="J146" t="s">
+        <v>62</v>
+      </c>
+      <c r="K146" t="s">
+        <v>62</v>
+      </c>
+      <c r="L146" t="s">
+        <v>32</v>
+      </c>
+      <c r="M146" t="s">
+        <v>33</v>
+      </c>
+      <c r="N146" t="s">
+        <v>34</v>
+      </c>
+      <c r="O146" t="s">
+        <v>35</v>
+      </c>
+      <c r="P146" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q146" t="s">
+        <v>63</v>
+      </c>
+      <c r="R146" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S146" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T146" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U146" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="147" spans="1:21">
+      <c r="A147" t="s">
+        <v>216</v>
+      </c>
+      <c r="B147" t="s">
+        <v>72</v>
+      </c>
+      <c r="C147" t="s">
+        <v>73</v>
+      </c>
+      <c r="D147" t="s">
+        <v>74</v>
+      </c>
+      <c r="E147" t="s">
+        <v>75</v>
+      </c>
+      <c r="F147" t="s">
+        <v>58</v>
+      </c>
+      <c r="G147" t="s">
+        <v>44</v>
+      </c>
+      <c r="H147" t="s">
+        <v>60</v>
+      </c>
+      <c r="I147" t="s">
+        <v>52</v>
+      </c>
+      <c r="J147" t="s">
+        <v>62</v>
+      </c>
+      <c r="K147" t="s">
+        <v>62</v>
+      </c>
+      <c r="L147" t="s">
+        <v>32</v>
+      </c>
+      <c r="M147" t="s">
+        <v>33</v>
+      </c>
+      <c r="N147" t="s">
+        <v>34</v>
+      </c>
+      <c r="O147" t="s">
+        <v>35</v>
+      </c>
+      <c r="P147" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q147" t="s">
+        <v>63</v>
+      </c>
+      <c r="R147" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S147" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T147" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U147" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="148" spans="1:21">
+      <c r="A148" t="s">
+        <v>217</v>
+      </c>
+      <c r="B148" t="s">
+        <v>72</v>
+      </c>
+      <c r="C148" t="s">
+        <v>73</v>
+      </c>
+      <c r="D148" t="s">
+        <v>74</v>
+      </c>
+      <c r="E148" t="s">
+        <v>75</v>
+      </c>
+      <c r="F148" t="s">
+        <v>58</v>
+      </c>
+      <c r="G148" t="s">
+        <v>59</v>
+      </c>
+      <c r="H148" t="s">
+        <v>45</v>
+      </c>
+      <c r="I148" t="s">
+        <v>52</v>
+      </c>
+      <c r="J148" t="s">
+        <v>62</v>
+      </c>
+      <c r="K148" t="s">
+        <v>62</v>
+      </c>
+      <c r="L148" t="s">
+        <v>32</v>
+      </c>
+      <c r="M148" t="s">
+        <v>33</v>
+      </c>
+      <c r="N148" t="s">
+        <v>34</v>
+      </c>
+      <c r="O148" t="s">
+        <v>35</v>
+      </c>
+      <c r="P148" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q148" t="s">
+        <v>63</v>
+      </c>
+      <c r="R148" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S148" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T148" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U148" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="149" spans="1:21">
+      <c r="A149" t="s">
+        <v>218</v>
+      </c>
+      <c r="B149" t="s">
+        <v>72</v>
+      </c>
+      <c r="C149" t="s">
+        <v>73</v>
+      </c>
+      <c r="D149" t="s">
+        <v>74</v>
+      </c>
+      <c r="E149" t="s">
+        <v>75</v>
+      </c>
+      <c r="F149" t="s">
+        <v>58</v>
+      </c>
+      <c r="G149" t="s">
+        <v>44</v>
+      </c>
+      <c r="H149" t="s">
+        <v>45</v>
+      </c>
+      <c r="I149" t="s">
+        <v>46</v>
+      </c>
+      <c r="J149" t="s">
+        <v>62</v>
+      </c>
+      <c r="K149" t="s">
+        <v>62</v>
+      </c>
+      <c r="L149" t="s">
+        <v>32</v>
+      </c>
+      <c r="M149" t="s">
+        <v>33</v>
+      </c>
+      <c r="N149" t="s">
+        <v>34</v>
+      </c>
+      <c r="O149" t="s">
+        <v>35</v>
+      </c>
+      <c r="P149" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q149" t="s">
+        <v>49</v>
+      </c>
+      <c r="R149" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S149" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T149" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U149" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="150" spans="1:21">
+      <c r="A150" t="s">
+        <v>219</v>
+      </c>
+      <c r="B150" t="s">
+        <v>72</v>
+      </c>
+      <c r="C150" t="s">
+        <v>73</v>
+      </c>
+      <c r="D150" t="s">
+        <v>74</v>
+      </c>
+      <c r="E150" t="s">
+        <v>75</v>
+      </c>
+      <c r="F150" t="s">
+        <v>58</v>
+      </c>
+      <c r="G150" t="s">
+        <v>44</v>
+      </c>
+      <c r="H150" t="s">
+        <v>60</v>
+      </c>
+      <c r="I150" t="s">
+        <v>46</v>
+      </c>
+      <c r="J150" t="s">
+        <v>62</v>
+      </c>
+      <c r="K150" t="s">
+        <v>62</v>
+      </c>
+      <c r="L150" t="s">
+        <v>32</v>
+      </c>
+      <c r="M150" t="s">
+        <v>33</v>
+      </c>
+      <c r="N150" t="s">
+        <v>34</v>
+      </c>
+      <c r="O150" t="s">
+        <v>35</v>
+      </c>
+      <c r="P150" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q150" t="s">
+        <v>49</v>
+      </c>
+      <c r="R150" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S150" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T150" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U150" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="151" spans="1:21">
+      <c r="A151" t="s">
+        <v>220</v>
+      </c>
+      <c r="B151" t="s">
+        <v>72</v>
+      </c>
+      <c r="C151" t="s">
+        <v>73</v>
+      </c>
+      <c r="D151" t="s">
+        <v>74</v>
+      </c>
+      <c r="E151" t="s">
+        <v>75</v>
+      </c>
+      <c r="F151" t="s">
+        <v>58</v>
+      </c>
+      <c r="G151" t="s">
+        <v>59</v>
+      </c>
+      <c r="H151" t="s">
+        <v>45</v>
+      </c>
+      <c r="I151" t="s">
+        <v>46</v>
+      </c>
+      <c r="J151" t="s">
+        <v>62</v>
+      </c>
+      <c r="K151" t="s">
+        <v>62</v>
+      </c>
+      <c r="L151" t="s">
+        <v>32</v>
+      </c>
+      <c r="M151" t="s">
+        <v>33</v>
+      </c>
+      <c r="N151" t="s">
+        <v>34</v>
+      </c>
+      <c r="O151" t="s">
+        <v>35</v>
+      </c>
+      <c r="P151" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q151" t="s">
+        <v>49</v>
+      </c>
+      <c r="R151" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S151" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T151" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U151" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="152" spans="1:21">
+      <c r="A152" t="s">
+        <v>221</v>
+      </c>
+      <c r="B152" t="s">
+        <v>72</v>
+      </c>
+      <c r="C152" t="s">
+        <v>73</v>
+      </c>
+      <c r="D152" t="s">
+        <v>74</v>
+      </c>
+      <c r="E152" t="s">
+        <v>75</v>
+      </c>
+      <c r="F152" t="s">
+        <v>58</v>
+      </c>
+      <c r="G152" t="s">
+        <v>44</v>
+      </c>
+      <c r="H152" t="s">
+        <v>45</v>
+      </c>
+      <c r="I152" t="s">
+        <v>52</v>
+      </c>
+      <c r="J152" t="s">
+        <v>62</v>
+      </c>
+      <c r="K152" t="s">
+        <v>62</v>
+      </c>
+      <c r="L152" t="s">
+        <v>32</v>
+      </c>
+      <c r="M152" t="s">
+        <v>33</v>
+      </c>
+      <c r="N152" t="s">
+        <v>34</v>
+      </c>
+      <c r="O152" t="s">
+        <v>35</v>
+      </c>
+      <c r="P152" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q152" t="s">
+        <v>49</v>
+      </c>
+      <c r="R152" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S152" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T152" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U152" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="153" spans="1:21">
+      <c r="A153" t="s">
+        <v>222</v>
+      </c>
+      <c r="B153" t="s">
+        <v>72</v>
+      </c>
+      <c r="C153" t="s">
+        <v>73</v>
+      </c>
+      <c r="D153" t="s">
+        <v>74</v>
+      </c>
+      <c r="E153" t="s">
+        <v>75</v>
+      </c>
+      <c r="F153" t="s">
+        <v>58</v>
+      </c>
+      <c r="G153" t="s">
+        <v>44</v>
+      </c>
+      <c r="H153" t="s">
+        <v>60</v>
+      </c>
+      <c r="I153" t="s">
+        <v>52</v>
+      </c>
+      <c r="J153" t="s">
+        <v>62</v>
+      </c>
+      <c r="K153" t="s">
+        <v>62</v>
+      </c>
+      <c r="L153" t="s">
+        <v>32</v>
+      </c>
+      <c r="M153" t="s">
+        <v>33</v>
+      </c>
+      <c r="N153" t="s">
+        <v>34</v>
+      </c>
+      <c r="O153" t="s">
+        <v>35</v>
+      </c>
+      <c r="P153" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q153" t="s">
+        <v>49</v>
+      </c>
+      <c r="R153" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S153" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T153" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U153" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="154" spans="1:21">
+      <c r="A154" t="s">
+        <v>223</v>
+      </c>
+      <c r="B154" t="s">
+        <v>72</v>
+      </c>
+      <c r="C154" t="s">
+        <v>73</v>
+      </c>
+      <c r="D154" t="s">
+        <v>74</v>
+      </c>
+      <c r="E154" t="s">
+        <v>75</v>
+      </c>
+      <c r="F154" t="s">
+        <v>58</v>
+      </c>
+      <c r="G154" t="s">
+        <v>59</v>
+      </c>
+      <c r="H154" t="s">
+        <v>45</v>
+      </c>
+      <c r="I154" t="s">
+        <v>52</v>
+      </c>
+      <c r="J154" t="s">
+        <v>62</v>
+      </c>
+      <c r="K154" t="s">
+        <v>62</v>
+      </c>
+      <c r="L154" t="s">
+        <v>32</v>
+      </c>
+      <c r="M154" t="s">
+        <v>33</v>
+      </c>
+      <c r="N154" t="s">
+        <v>34</v>
+      </c>
+      <c r="O154" t="s">
+        <v>35</v>
+      </c>
+      <c r="P154" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q154" t="s">
+        <v>49</v>
+      </c>
+      <c r="R154" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S154" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T154" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="U154" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="155" spans="1:21" s="1" customFormat="1">
+      <c r="A155" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="B155" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="C155" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D104" s="1" t="s">
+      <c r="D155" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E104" s="1" t="s">
+      <c r="E155" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F104" s="1" t="s">
+      <c r="F155" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G104" s="1" t="s">
+      <c r="G155" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H104" s="1" t="s">
+      <c r="H155" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I104" s="1" t="s">
+      <c r="I155" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J104" s="1" t="s">
+      <c r="J155" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K104" s="1" t="s">
+      <c r="K155" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L104" s="1" t="s">
+      <c r="L155" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M104" s="1" t="s">
+      <c r="M155" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N104" s="1" t="s">
+      <c r="N155" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O104" s="1" t="s">
+      <c r="O155" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P104" s="1" t="s">
+      <c r="P155" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q104" s="1" t="s">
+      <c r="Q155" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R104" s="1" t="s">
+      <c r="R155" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S104" s="1" t="s">
+      <c r="S155" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T104" s="1" t="s">
+      <c r="T155" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U104" s="1" t="s">
+      <c r="U155" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="105" spans="1:21" s="1" customFormat="1">
-      <c r="Q105" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="R105" s="1">
+    <row r="156" spans="1:21" s="1" customFormat="1">
+      <c r="Q156" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="R156" s="1">
         <v>250.514</v>
       </c>
-      <c r="S105" s="1">
+      <c r="S156" s="1">
         <v>-99.48650000000001</v>
       </c>
-      <c r="T105" s="1">
+      <c r="T156" s="1">
         <v>-17.5226</v>
       </c>
-      <c r="U105" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="106" spans="1:21" s="1" customFormat="1">
-      <c r="Q106" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="R106" s="1">
+      <c r="U156" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="157" spans="1:21" s="1" customFormat="1">
+      <c r="Q157" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="R157" s="1">
         <v>267.523</v>
       </c>
-      <c r="S106" s="1">
+      <c r="S157" s="1">
         <v>-47.4774</v>
       </c>
-      <c r="T106" s="1">
+      <c r="T157" s="1">
         <v>-0.513522</v>
       </c>
-      <c r="U106" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="107" spans="1:21" s="1" customFormat="1">
-      <c r="Q107" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="108" spans="1:21" s="1" customFormat="1">
-      <c r="Q108" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="109" spans="1:21" s="1" customFormat="1">
-      <c r="Q109" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="110" spans="1:21" s="1" customFormat="1">
-      <c r="Q110" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="111" spans="1:21" s="1" customFormat="1">
-      <c r="Q111" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="R111" s="1">
+      <c r="U157" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="158" spans="1:21" s="1" customFormat="1">
+      <c r="Q158" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="159" spans="1:21" s="1" customFormat="1">
+      <c r="Q159" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="160" spans="1:21" s="1" customFormat="1">
+      <c r="Q160" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="161" spans="17:21" s="1" customFormat="1">
+      <c r="Q161" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="162" spans="17:21" s="1" customFormat="1">
+      <c r="Q162" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="R162" s="1">
         <v>256.26</v>
       </c>
-      <c r="S111" s="1">
+      <c r="S162" s="1">
         <v>-70.40703000000001</v>
       </c>
-      <c r="T111" s="1">
+      <c r="T162" s="1">
         <v>-6.259639</v>
       </c>
-      <c r="U111" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="112" spans="1:21" s="1" customFormat="1">
-      <c r="Q112" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="R112" s="1">
+      <c r="U162" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="163" spans="17:21" s="1" customFormat="1">
+      <c r="Q163" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="R163" s="1">
         <v>7.964692</v>
       </c>
-      <c r="S112" s="1">
+      <c r="S163" s="1">
         <v>21.673362</v>
       </c>
-      <c r="T112" s="1">
+      <c r="T163" s="1">
         <v>7.964666</v>
       </c>
-      <c r="U112" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="113" spans="17:21" s="1" customFormat="1">
-      <c r="Q113" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="R113" s="1">
+      <c r="U163" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="164" spans="17:21" s="1" customFormat="1">
+      <c r="Q164" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="R164" s="1">
         <v>3.108051</v>
       </c>
-      <c r="S113" s="1">
+      <c r="S164" s="1">
         <v>30.782952</v>
       </c>
-      <c r="T113" s="1">
+      <c r="T164" s="1">
         <v>127.238424</v>
       </c>
-      <c r="U113" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="114" spans="17:21" s="1" customFormat="1"/>
+      <c r="U164" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="165" spans="17:21" s="1" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>